<commit_message>
✨ adding support for text border
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Repositories\BannerCreator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B55810-7B1C-4AC5-851D-CFB5BC8F5E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86D740B-F691-456D-932F-19C4D323862E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Group</t>
   </si>
@@ -49,20 +49,29 @@
     <t>#FF414D</t>
   </si>
   <si>
-    <t>../public/Plantillas/Bandera.png</t>
-  </si>
-  <si>
     <t>./asset/font/Sportage-DemoItalic.otf</t>
   </si>
   <si>
     <t>1450 Bs</t>
+  </si>
+  <si>
+    <t>../public/in/Caminito.JPG</t>
+  </si>
+  <si>
+    <t>Border</t>
+  </si>
+  <si>
+    <t>Bordercolor</t>
+  </si>
+  <si>
+    <t>#F7CD31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -77,6 +86,17 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -120,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,6 +148,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,21 +467,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="25.08984375" customWidth="1"/>
-    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="10" max="10" width="25.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,19 +500,24 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>500</v>
@@ -505,26 +531,32 @@
       <c r="F2" s="2">
         <v>200</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3">
+        <v>50</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -532,10 +564,11 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -545,8 +578,9 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -556,8 +590,9 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -567,8 +602,9 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -578,8 +614,9 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -589,8 +626,9 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -600,8 +638,9 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -611,8 +650,9 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -622,8 +662,9 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -633,8 +674,9 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -644,8 +686,9 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -655,8 +698,9 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -666,8 +710,10 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
⚡ Adding Example Data
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Repositories\BannerCreator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86D740B-F691-456D-932F-19C4D323862E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9968DDD-8ABB-43A8-ABEC-4BBEF9803AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Group</t>
   </si>
@@ -46,25 +46,28 @@
     <t>Fonttype</t>
   </si>
   <si>
-    <t>#FF414D</t>
-  </si>
-  <si>
     <t>./asset/font/Sportage-DemoItalic.otf</t>
   </si>
   <si>
-    <t>1450 Bs</t>
-  </si>
-  <si>
-    <t>../public/in/Caminito.JPG</t>
-  </si>
-  <si>
     <t>Border</t>
   </si>
   <si>
     <t>Bordercolor</t>
   </si>
   <si>
-    <t>#F7CD31</t>
+    <t>./asset/image/example.image.jpg</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>#EC3C66</t>
   </si>
 </sst>
 </file>
@@ -469,8 +472,8 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -500,10 +503,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -517,44 +520,64 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3">
+        <v>100</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2">
+        <v>150</v>
+      </c>
+      <c r="G2" s="3">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
-        <v>500</v>
-      </c>
-      <c r="D2" s="2">
-        <v>580</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2">
-        <v>200</v>
-      </c>
-      <c r="G2" s="3">
-        <v>50</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3">
+        <v>200</v>
+      </c>
+      <c r="D3" s="3">
+        <v>300</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3">
+        <v>120</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>

</xml_diff>

<commit_message>
⚡ creating run file ⚡ updating config path to match with path of run file
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Repositories\BannerCreator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9968DDD-8ABB-43A8-ABEC-4BBEF9803AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438EDA20-CA48-40D1-A0FE-C3A8EA45B3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -46,18 +46,12 @@
     <t>Fonttype</t>
   </si>
   <si>
-    <t>./asset/font/Sportage-DemoItalic.otf</t>
-  </si>
-  <si>
     <t>Border</t>
   </si>
   <si>
     <t>Bordercolor</t>
   </si>
   <si>
-    <t>./asset/image/example.image.jpg</t>
-  </si>
-  <si>
     <t>#FFFFFF</t>
   </si>
   <si>
@@ -68,6 +62,12 @@
   </si>
   <si>
     <t>#EC3C66</t>
+  </si>
+  <si>
+    <t>./src/asset/image/example.image.jpg</t>
+  </si>
+  <si>
+    <t>./src/asset/font/Sportage-DemoItalic.otf</t>
   </si>
 </sst>
 </file>
@@ -472,15 +472,15 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
-    <col min="10" max="10" width="25.08984375" customWidth="1"/>
+    <col min="10" max="10" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -503,10 +503,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>100</v>
@@ -529,7 +529,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2">
         <v>150</v>
@@ -538,13 +538,13 @@
         <v>10</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3">
         <v>200</v>
@@ -561,7 +561,7 @@
         <v>300</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3">
         <v>120</v>
@@ -570,13 +570,13 @@
         <v>5</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
⚡ updating example image ➕ adding to track an example output image
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Repositories\BannerCreator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438EDA20-CA48-40D1-A0FE-C3A8EA45B3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049C3B39-3709-4421-8E9E-88864955A9E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Group</t>
   </si>
@@ -55,12 +55,6 @@
     <t>#FFFFFF</t>
   </si>
   <si>
-    <t>Welcome</t>
-  </si>
-  <si>
-    <t>Users</t>
-  </si>
-  <si>
     <t>#EC3C66</t>
   </si>
   <si>
@@ -68,13 +62,22 @@
   </si>
   <si>
     <t>./src/asset/font/Sportage-DemoItalic.otf</t>
+  </si>
+  <si>
+    <t>That's just</t>
+  </si>
+  <si>
+    <t>An Example Image</t>
+  </si>
+  <si>
+    <t>#00FFCC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -98,6 +101,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -473,13 +481,13 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="9" max="9" width="32.26953125" customWidth="1"/>
     <col min="10" max="10" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -520,31 +528,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D2" s="3">
         <v>100</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="G2" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -552,19 +560,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="D3" s="3">
         <v>300</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G3" s="3">
         <v>5</v>
@@ -573,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -736,6 +744,7 @@
       <c r="J16" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Adding new Centering Argument on Config Example File
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Repositories\BannerCreator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Repositories\CadeSur\BannerCreator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049C3B39-3709-4421-8E9E-88864955A9E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC87D27A-D212-48C8-B839-2A23AC087E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31650" yWindow="2850" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Group</t>
   </si>
@@ -67,10 +67,21 @@
     <t>That's just</t>
   </si>
   <si>
-    <t>An Example Image</t>
-  </si>
-  <si>
     <t>#00FFCC</t>
+  </si>
+  <si>
+    <t>Centering</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>yx</t>
+  </si>
+  <si>
+    <t>An Example Image 
+sdfgfhgjfhg,j.h,ghghfg
+test</t>
   </si>
 </sst>
 </file>
@@ -151,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,6 +172,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,20 +492,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="9" max="9" width="32.26953125" customWidth="1"/>
-    <col min="10" max="10" width="35.81640625" customWidth="1"/>
+    <col min="9" max="10" width="32.26953125" customWidth="1"/>
+    <col min="11" max="11" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,10 +534,13 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -552,15 +569,18 @@
         <v>12</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C3" s="3">
         <v>80</v>
@@ -569,7 +589,7 @@
         <v>300</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3">
         <v>80</v>
@@ -584,10 +604,13 @@
         <v>12</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -598,8 +621,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -610,8 +634,9 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -622,8 +647,9 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -634,8 +660,9 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -646,8 +673,9 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -658,8 +686,9 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -670,8 +699,9 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -682,8 +712,9 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -694,8 +725,9 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -706,8 +738,9 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -718,8 +751,9 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -730,8 +764,9 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -742,6 +777,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>